<commit_message>
edit some code rows
</commit_message>
<xml_diff>
--- a/tables_work/main_task/recipes_model.xlsx
+++ b/tables_work/main_task/recipes_model.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\3_КУРС_СЕМИНАРЫ\ТОБД\6_сем\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6FFCF3-6995-4CEE-B980-2C106778F976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE79B1E1-17B2-4683-9CF9-E5A9B04F3DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12288" yWindow="1212" windowWidth="17268" windowHeight="11052" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11184" yWindow="1236" windowWidth="17268" windowHeight="11052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Модель" sheetId="1" r:id="rId1"/>
-    <sheet name="Ошибки заполнения" sheetId="3" r:id="rId2"/>
-    <sheet name="Статистика" sheetId="5" r:id="rId3"/>
+    <sheet name="Статистика" sheetId="3" r:id="rId1"/>
+    <sheet name="Ошибки заполнения" sheetId="2" r:id="rId2"/>
+    <sheet name="Модель" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Модель!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Модель!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -337,21 +337,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>335289</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>89922</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>51822</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="MyPlot">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57411CB1-3781-73FF-DF8A-3738027C395D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26FA1E23-27EC-99EA-C36C-319FFB418812}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -373,7 +373,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="952500"/>
+          <a:off x="0" y="1097280"/>
           <a:ext cx="4602489" cy="3160782"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -706,12 +706,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBED10D-61BB-4B72-802B-FB6013B06395}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083856A3-6A24-4232-88C6-DF0573E0FF0C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
-    </sheetView>
+    <sheetView topLeftCell="F1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1213,143 +1350,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83FDF6F7-B9F5-42D6-8D59-09ED0D75B2B4}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727B4247-B30C-4313-96B6-BF2F92C19DA8}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>